<commit_message>
task and table màj
</commit_message>
<xml_diff>
--- a/todo/task.xlsx
+++ b/todo/task.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t xml:space="preserve">Conception base (2h) :</t>
   </si>
@@ -82,10 +82,10 @@
     <t xml:space="preserve">Accueil Admin </t>
   </si>
   <si>
-    <t xml:space="preserve">accueilAdmin.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt; accueil avec nav bar : variété - parcelles – cueilleurs – catDépenses</t>
+    <t xml:space="preserve">(ok) accueilAdmin.html (1h30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; accueil avec nav bar : variété - parcelles – cueilleurs – catDépenses – salKilo</t>
   </si>
   <si>
     <t xml:space="preserve">&gt; css affichage </t>
@@ -97,10 +97,31 @@
     <t xml:space="preserve">&gt; fonction généralisé selectAll </t>
   </si>
   <si>
-    <t xml:space="preserve">.</t>
+    <t xml:space="preserve">&gt; modele_accueil.Admin.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; folder : type Gestion ; page : insert ou list</t>
   </si>
   <si>
     <t xml:space="preserve">&gt; rediriger vers les bonnes pages de crud </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type Gestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; formulaire de chq entité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; getListeVariete by Parcelle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; fonction js : displayInTable (tabObject) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; traitement AJAX pour chaque insertion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; traitement AJAX pour list entité</t>
   </si>
 </sst>
 </file>
@@ -218,10 +239,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D49" activeCellId="0" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -408,14 +429,64 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D39" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="0" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D41" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D45" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D48" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D49" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D52" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D53" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User Choice and Log User Lambda
</commit_message>
<xml_diff>
--- a/todo/task.xlsx
+++ b/todo/task.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
   <si>
     <t xml:space="preserve">Conception base (2h) :</t>
   </si>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">Choix Connection</t>
   </si>
   <si>
-    <t xml:space="preserve">choixConnect.html</t>
+    <t xml:space="preserve">choixConnect.html (20mn)</t>
   </si>
   <si>
     <t xml:space="preserve">&gt; lien : Admin ou Utilisateur Lambda</t>
@@ -139,13 +139,13 @@
     <t xml:space="preserve">&gt; rediriger les liens </t>
   </si>
   <si>
-    <t xml:space="preserve">logUser.php </t>
+    <t xml:space="preserve">logUser.php (1h)</t>
   </si>
   <si>
     <t xml:space="preserve">&gt; envoyer données formulaire vers traitLogUser.php</t>
   </si>
   <si>
-    <t xml:space="preserve">traitLogUser.php</t>
+    <t xml:space="preserve">traitLogUser.php (30mn)</t>
   </si>
   <si>
     <t xml:space="preserve">&gt; fonction verifLogUtilisateur</t>
@@ -232,7 +232,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -246,10 +246,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -272,8 +268,8 @@
   </sheetPr>
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C85" activeCellId="4" sqref="C67:C68 C74 C80:C82 C84 C85"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J71" activeCellId="0" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -562,7 +558,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -572,6 +568,9 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="D59" s="0" t="s">
         <v>36</v>
       </c>
@@ -582,6 +581,9 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C62" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="D62" s="0" t="s">
         <v>38</v>
       </c>
@@ -600,11 +602,17 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="D67" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="D68" s="2" t="s">
         <v>7</v>
       </c>
@@ -627,6 +635,9 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C74" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="D74" s="2" t="s">
         <v>40</v>
       </c>
@@ -655,11 +666,17 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C81" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="E81" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C82" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="E82" s="0" t="s">
         <v>15</v>
       </c>
@@ -670,11 +687,17 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C84" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="D84" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C85" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="D85" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Insertion The_Saison et The_MoisSaison
</commit_message>
<xml_diff>
--- a/todo/task.xlsx
+++ b/todo/task.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="94">
   <si>
     <t xml:space="preserve">Conception base (2h) :</t>
   </si>
@@ -283,7 +283,7 @@
     <t xml:space="preserve">The_MoisSaison : id – idSaison – numMois </t>
   </si>
   <si>
-    <t xml:space="preserve">configSaison.html</t>
+    <t xml:space="preserve">configSaison.html (2h)</t>
   </si>
   <si>
     <t xml:space="preserve">&gt; ajout lien bar de navigation : saison </t>
@@ -385,7 +385,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -395,10 +395,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -421,8 +417,8 @@
   </sheetPr>
   <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D163" activeCellId="0" sqref="D163"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A145" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B154" activeCellId="0" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1191,7 +1187,7 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C144" s="0" t="s">
+      <c r="C144" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D144" s="2" t="s">
@@ -1199,7 +1195,7 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C145" s="0" t="s">
+      <c r="C145" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D145" s="2" t="s">
@@ -1207,77 +1203,101 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="3" t="s">
+      <c r="A147" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="3"/>
+      <c r="A148" s="1"/>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="3"/>
-      <c r="B149" s="0" t="s">
+      <c r="A149" s="1"/>
+      <c r="B149" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="3"/>
-      <c r="C150" s="0" t="s">
+      <c r="A150" s="1"/>
+      <c r="B150" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C151" s="0" t="s">
+      <c r="B151" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C151" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B153" s="0" t="s">
+      <c r="B153" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C154" s="0" t="s">
+      <c r="C154" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D155" s="0" t="s">
+      <c r="B155" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D155" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D156" s="0" t="s">
+      <c r="B156" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D156" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E157" s="0" t="s">
+      <c r="B157" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E157" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E158" s="0" t="s">
+      <c r="B158" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E158" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C159" s="0" t="s">
+      <c r="C159" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D160" s="0" t="s">
+      <c r="B160" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D160" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C162" s="0" t="s">
+      <c r="C162" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D163" s="0" t="s">
+      <c r="B163" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D163" s="2" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>